<commit_message>
DB Design document updated
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773CC616-7D00-4CE4-84A2-79FEC98E36AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C6E1F-9C87-4A53-BD15-E53407F64939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="106">
   <si>
     <t>Created By</t>
   </si>
@@ -156,9 +156,6 @@
     <t>USER_EMAIL_ID</t>
   </si>
   <si>
-    <t>VACCINE_NO_OF_DOSES</t>
-  </si>
-  <si>
     <t>NUMBER (2)</t>
   </si>
   <si>
@@ -292,6 +289,63 @@
   </si>
   <si>
     <t>ILLNESS_ISOTHER</t>
+  </si>
+  <si>
+    <t>USER_ALLERGIC_CONDITIONS</t>
+  </si>
+  <si>
+    <t>USER_ALLGCOND_ID</t>
+  </si>
+  <si>
+    <t>REFERENCE TO ALLGCOND_ID OF ALLERGIC_CONDITIONS_MASTER</t>
+  </si>
+  <si>
+    <t>USER_ILLNESS</t>
+  </si>
+  <si>
+    <t>USER_ILLNESS_ID</t>
+  </si>
+  <si>
+    <t>REFERENCE TO ILLNESS_ID OF ILLNESS_MASTER</t>
+  </si>
+  <si>
+    <t>VACCINE_DOSE_MASTER</t>
+  </si>
+  <si>
+    <t>VACCINE_DOSE_ID</t>
+  </si>
+  <si>
+    <t>VACCINE_DOSE_NAME</t>
+  </si>
+  <si>
+    <t>VACCINE_DOSE_DETAIL</t>
+  </si>
+  <si>
+    <t>VACCINE_DOSE_ISACTIVE</t>
+  </si>
+  <si>
+    <t>REFERENCE TOVACCINE_ID OF VACCINE_MASTER TABLE</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_TITLE_ID</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_FIRST_NAME</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_MIDDLE_NAME</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_LAST_NAME</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_MOBILE_NUMBER</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_ALTERNATE_NUMBER</t>
+  </si>
+  <si>
+    <t>USER_REPORTER_EMAIL_ID</t>
   </si>
 </sst>
 </file>
@@ -744,7 +798,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:D2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,10 +845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4501CC-882B-43D3-A85F-1FC8AD5DCF77}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,10 +924,10 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="8" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
@@ -882,19 +936,19 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>15</v>
@@ -903,53 +957,57 @@
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>33</v>
-      </c>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
@@ -958,19 +1016,19 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>15</v>
@@ -979,41 +1037,41 @@
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="8" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="8"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="8" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
@@ -1022,7 +1080,7 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="8" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>23</v>
@@ -1057,10 +1115,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>10</v>
@@ -1070,75 +1128,47 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="H23" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-    </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>69</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="8" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>15</v>
@@ -1146,67 +1176,87 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="8" t="s">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="8"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="10"/>
+      <c r="H30" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+    </row>
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="8" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>15</v>
@@ -1214,75 +1264,83 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="8" t="s">
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="8"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="8" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
       <c r="B40" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>15</v>
@@ -1291,27 +1349,104 @@
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="8" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10"/>
+      <c r="C48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="H23:K27"/>
-    <mergeCell ref="A29:A33"/>
+  <mergeCells count="8">
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="H30:K34"/>
+    <mergeCell ref="A36:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1319,15 +1454,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F028140-CA34-4194-A102-025CA8E62727}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
@@ -1474,10 +1609,10 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -1486,7 +1621,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>10</v>
@@ -1498,7 +1633,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>15</v>
@@ -1510,191 +1645,425 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="14" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
+        <v>10</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="14" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="14" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="15"/>
       <c r="F18" s="16"/>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+    </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>46</v>
-      </c>
+      <c r="A21" s="12"/>
       <c r="B21" s="14" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>11</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D21" s="14"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="14" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+        <v>13</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
       <c r="B23" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="14" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
       <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="14" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
-    </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="B28" s="14" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="E28" s="15"/>
       <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
+      <c r="C36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="A21:A29"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A44:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1704,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3ACC7-C065-475E-9BD1-DEB1E2424B3A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
DB Design Document Updated with almost all the possible tables
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C6E1F-9C87-4A53-BD15-E53407F64939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F47BED-4567-469F-8940-06A77AA799C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="123">
   <si>
     <t>Created By</t>
   </si>
@@ -156,9 +156,6 @@
     <t>USER_EMAIL_ID</t>
   </si>
   <si>
-    <t>NUMBER (2)</t>
-  </si>
-  <si>
     <t>USER_ADDRESS</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>SELF, HEALTHCARE_PROFESSIONAL, RELATIVE, OTHERS</t>
   </si>
   <si>
-    <t>USVAC_VACCINATION_DOSE_NUMBER</t>
-  </si>
-  <si>
     <t>USER_AGE</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t xml:space="preserve">There will be multiple entries for each Adverse Event in this table since the underlying adverse events can be same for two Root level adverse events. For example, Head-ache is common for Fever and Vomiting </t>
   </si>
   <si>
-    <t>ADEV_IS_ROOT_ELEMENT</t>
-  </si>
-  <si>
     <t>USER_SEX</t>
   </si>
   <si>
@@ -346,6 +337,66 @@
   </si>
   <si>
     <t>USER_REPORTER_EMAIL_ID</t>
+  </si>
+  <si>
+    <t>USVAC_VACCINE_DOSE_ID</t>
+  </si>
+  <si>
+    <t>REFERENCE TO VACCINE_DOSE_ID OF VACCINE_DOSE_MASTER TABLE</t>
+  </si>
+  <si>
+    <t>ADVERSE_EVENT_REPORTED</t>
+  </si>
+  <si>
+    <t>ADEV_REP_ID</t>
+  </si>
+  <si>
+    <t>REFERENCE TO USVAC_ID OF USER_VACCINE TABLE</t>
+  </si>
+  <si>
+    <t>ADEV_IS_PARENT_ELEMENT</t>
+  </si>
+  <si>
+    <t>This should contain the ID of the Adverse_Event_Master entries in which the ADEV_IS_PARENT_ELEMENT is TRUE</t>
+  </si>
+  <si>
+    <t>This should contain the ID of the Adverse_Event_Master entries in which the ADEV_IS_PARENT_ELEMENT is FALSE</t>
+  </si>
+  <si>
+    <t>CLOB</t>
+  </si>
+  <si>
+    <t>ADEV_REP_PARENT_ADEV_ID</t>
+  </si>
+  <si>
+    <t>ADEV_REP_USVAC_ID</t>
+  </si>
+  <si>
+    <t>ADEV_REP_CHILD_ADEV_ID</t>
+  </si>
+  <si>
+    <t>ADEV_REP_ADDITIONAL_NOTES</t>
+  </si>
+  <si>
+    <t>ADEV_REP_DATE_TIME</t>
+  </si>
+  <si>
+    <t>ADEV_REP_ISFATAL</t>
+  </si>
+  <si>
+    <t>ADEV_REP_DATE_OF_DEATH</t>
+  </si>
+  <si>
+    <t>ADEV_REP_ISMEDIC_NEEDED</t>
+  </si>
+  <si>
+    <t>ADEV_REP_MEDIC_NOTES</t>
+  </si>
+  <si>
+    <t>ADEV_REP_ISRECOVERED</t>
+  </si>
+  <si>
+    <t>ADEV_REP_RECOVERY_DATE</t>
   </si>
 </sst>
 </file>
@@ -847,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4501CC-882B-43D3-A85F-1FC8AD5DCF77}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,10 +1010,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -985,14 +1036,14 @@
         <v>32</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>13</v>
@@ -1004,10 +1055,10 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
@@ -1016,7 +1067,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>23</v>
@@ -1115,10 +1166,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>10</v>
@@ -1132,7 +1183,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
@@ -1144,7 +1195,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="8" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>23</v>
@@ -1156,7 +1207,7 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>23</v>
@@ -1191,10 +1242,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>10</v>
@@ -1205,7 +1256,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="10"/>
       <c r="H30" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -1214,7 +1265,7 @@
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>10</v>
@@ -1223,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F31" s="9"/>
       <c r="H31" s="20"/>
@@ -1234,7 +1285,7 @@
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>10</v>
@@ -1243,10 +1294,10 @@
         <v>32</v>
       </c>
       <c r="E32" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
@@ -1287,10 +1338,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>10</v>
@@ -1304,7 +1355,7 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>35</v>
@@ -1316,7 +1367,7 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
       <c r="B38" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>23</v>
@@ -1351,10 +1402,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>10</v>
@@ -1368,7 +1419,7 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>35</v>
@@ -1380,7 +1431,7 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>23</v>
@@ -1392,7 +1443,7 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
@@ -1404,7 +1455,7 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
@@ -1456,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F028140-CA34-4194-A102-025CA8E62727}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,10 +1660,10 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
@@ -1621,7 +1672,7 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>10</v>
@@ -1633,7 +1684,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>15</v>
@@ -1645,63 +1696,63 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="14" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D15" s="14"/>
-      <c r="E15" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="E15" s="15"/>
       <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="14" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>32</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+        <v>10</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>13</v>
@@ -1713,7 +1764,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>13</v>
@@ -1725,10 +1776,10 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
@@ -1737,7 +1788,7 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>39</v>
@@ -1749,10 +1800,10 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
@@ -1761,10 +1812,10 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="14" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
@@ -1773,19 +1824,19 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="14" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
       <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>15</v>
@@ -1794,42 +1845,38 @@
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="16"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="14" t="s">
+      <c r="C29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E29" s="15"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>10</v>
@@ -1838,41 +1885,49 @@
         <v>32</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
-      <c r="B32" s="14" t="s">
-        <v>52</v>
+      <c r="B32" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="15"/>
+        <v>10</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="15"/>
@@ -1881,10 +1936,10 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="14" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="15"/>
@@ -1916,10 +1971,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>10</v>
@@ -1933,7 +1988,7 @@
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>10</v>
@@ -1942,7 +1997,7 @@
         <v>32</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F39" s="9"/>
     </row>
@@ -1958,7 +2013,7 @@
         <v>32</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F40" s="10"/>
     </row>
@@ -1988,10 +2043,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>10</v>
@@ -2005,7 +2060,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>10</v>
@@ -2014,7 +2069,7 @@
         <v>32</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F45" s="9"/>
     </row>
@@ -2030,7 +2085,7 @@
         <v>32</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="10"/>
     </row>
@@ -2060,8 +2115,8 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A2:A26"/>
+    <mergeCell ref="A29:A36"/>
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A44:A48"/>
   </mergeCells>
@@ -2071,12 +2126,234 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3ACC7-C065-475E-9BD1-DEB1E2424B3A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
+    <col min="6" max="6" width="63.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit of the Project Structure with Vaccine Master GET API
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B270DD-086F-4B47-97B3-5658820A993E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF0A628-C529-439C-8B1F-584755CA0146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,18 @@
     <sheet name="User Tables" sheetId="3" r:id="rId3"/>
     <sheet name="Adverse Event Tables" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -249,9 +257,6 @@
     <t>USER_DOB</t>
   </si>
   <si>
-    <t>USVAC_IS_PREGNANT</t>
-  </si>
-  <si>
     <t>ALLERGIC_CONDITIONS_MASTER</t>
   </si>
   <si>
@@ -397,13 +402,16 @@
   </si>
   <si>
     <t>ADEV_REP_START_DATE_TIME</t>
+  </si>
+  <si>
+    <t>USER_IS_PREGNANT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,8 +427,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,8 +459,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -506,11 +526,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,6 +574,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -557,6 +600,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,6 +614,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -898,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4501CC-882B-43D3-A85F-1FC8AD5DCF77}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +964,7 @@
     <col min="6" max="6" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -932,8 +984,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -947,9 +999,10 @@
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
@@ -959,9 +1012,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
       <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
@@ -971,9 +1025,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
       <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
@@ -983,9 +1038,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -995,9 +1051,10 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1007,13 +1064,14 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="G7" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -1023,9 +1081,10 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1036,14 +1095,15 @@
         <v>32</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
       <c r="B11" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>13</v>
@@ -1051,11 +1111,12 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
       <c r="B12" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>52</v>
@@ -1063,11 +1124,12 @@
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
       <c r="B13" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>23</v>
@@ -1075,9 +1137,10 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1087,9 +1150,10 @@
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
@@ -1099,9 +1163,10 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1115,9 +1180,10 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
+      <c r="G17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
@@ -1127,9 +1193,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
+      <c r="G18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
@@ -1139,9 +1206,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
+      <c r="G19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1151,9 +1219,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
+      <c r="G20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="8" t="s">
         <v>16</v>
       </c>
@@ -1163,9 +1232,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1179,9 +1249,10 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="8" t="s">
         <v>61</v>
       </c>
@@ -1191,21 +1262,23 @@
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
       <c r="B25" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="24"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="8" t="s">
         <v>62</v>
       </c>
@@ -1215,9 +1288,10 @@
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
+      <c r="G26" s="24"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="8" t="s">
         <v>14</v>
       </c>
@@ -1227,9 +1301,10 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="8" t="s">
         <v>16</v>
       </c>
@@ -1239,9 +1314,10 @@
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="10"/>
+      <c r="G28" s="24"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -1255,15 +1331,16 @@
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="10"/>
-      <c r="H30" s="14" t="s">
+      <c r="G30" s="25"/>
+      <c r="H30" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="8" t="s">
         <v>65</v>
       </c>
@@ -1277,13 +1354,14 @@
         <v>66</v>
       </c>
       <c r="F31" s="9"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="8" t="s">
         <v>67</v>
       </c>
@@ -1299,13 +1377,14 @@
       <c r="F32" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -1315,13 +1394,14 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="8" t="s">
         <v>16</v>
       </c>
@@ -1331,17 +1411,18 @@
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>10</v>
@@ -1351,11 +1432,12 @@
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
+      <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>35</v>
@@ -1363,11 +1445,12 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
+      <c r="G37" s="24"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>23</v>
@@ -1375,9 +1458,10 @@
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
+      <c r="G38" s="24"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="8" t="s">
         <v>14</v>
       </c>
@@ -1387,9 +1471,10 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
+      <c r="G39" s="24"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="8" t="s">
         <v>16</v>
       </c>
@@ -1399,13 +1484,14 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>10</v>
@@ -1415,11 +1501,12 @@
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>35</v>
@@ -1427,11 +1514,12 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>23</v>
@@ -1439,11 +1527,12 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
@@ -1451,11 +1540,12 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
+      <c r="G45" s="24"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
@@ -1463,9 +1553,10 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
+      <c r="G46" s="24"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -1475,9 +1566,10 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
@@ -1487,9 +1579,10 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
+      <c r="G48" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
     <mergeCell ref="H30:K34"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="A42:A48"/>
@@ -1498,17 +1591,25 @@
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A23:A28"/>
     <mergeCell ref="A30:A34"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G9:G15"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G42:G48"/>
+    <mergeCell ref="G30:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F028140-CA34-4194-A102-025CA8E62727}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1622,7 @@
     <col min="6" max="6" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1541,8 +1642,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1556,9 +1657,10 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
       <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1568,9 +1670,10 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
       <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
@@ -1584,9 +1687,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
@@ -1596,9 +1700,10 @@
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
       <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
@@ -1608,9 +1713,10 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
       <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
@@ -1620,9 +1726,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
       <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
@@ -1632,9 +1739,10 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
       <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
@@ -1644,9 +1752,10 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
@@ -1656,9 +1765,10 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
       <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
@@ -1668,9 +1778,10 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
       <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
@@ -1680,9 +1791,10 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
       <c r="B13" s="11" t="s">
         <v>72</v>
       </c>
@@ -1692,9 +1804,10 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
       <c r="B14" s="11" t="s">
         <v>70</v>
       </c>
@@ -1706,11 +1819,12 @@
         <v>71</v>
       </c>
       <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="11" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>23</v>
@@ -1718,9 +1832,10 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
       <c r="B16" s="11" t="s">
         <v>55</v>
       </c>
@@ -1732,11 +1847,12 @@
         <v>57</v>
       </c>
       <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
       <c r="B17" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>10</v>
@@ -1748,11 +1864,12 @@
         <v>37</v>
       </c>
       <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
       <c r="B18" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>13</v>
@@ -1760,11 +1877,12 @@
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
       <c r="B19" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>13</v>
@@ -1772,11 +1890,12 @@
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
       <c r="B20" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>13</v>
@@ -1784,11 +1903,12 @@
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
       <c r="B21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>39</v>
@@ -1796,11 +1916,12 @@
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
       <c r="B22" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>39</v>
@@ -1808,11 +1929,12 @@
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
       <c r="B23" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>13</v>
@@ -1820,9 +1942,10 @@
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
       <c r="B24" s="11" t="s">
         <v>50</v>
       </c>
@@ -1832,9 +1955,10 @@
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
       <c r="B25" s="11" t="s">
         <v>14</v>
       </c>
@@ -1844,9 +1968,10 @@
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
       <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
@@ -1856,9 +1981,10 @@
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="G26" s="24"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1872,9 +1998,10 @@
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="27"/>
       <c r="B30" s="11" t="s">
         <v>46</v>
       </c>
@@ -1888,9 +2015,10 @@
         <v>47</v>
       </c>
       <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
       <c r="B31" s="11" t="s">
         <v>48</v>
       </c>
@@ -1904,11 +2032,12 @@
         <v>49</v>
       </c>
       <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
       <c r="B32" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>10</v>
@@ -1917,12 +2046,13 @@
         <v>32</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F32" s="13"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
       <c r="B33" s="11" t="s">
         <v>53</v>
       </c>
@@ -1932,9 +2062,10 @@
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="27"/>
       <c r="B34" s="11" t="s">
         <v>51</v>
       </c>
@@ -1944,9 +2075,10 @@
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="27"/>
       <c r="B35" s="11" t="s">
         <v>14</v>
       </c>
@@ -1956,9 +2088,10 @@
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
       <c r="B36" s="11" t="s">
         <v>16</v>
       </c>
@@ -1968,13 +2101,14 @@
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="G36" s="24"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>10</v>
@@ -1984,11 +2118,12 @@
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
       <c r="B39" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>10</v>
@@ -1997,12 +2132,13 @@
         <v>32</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
       </c>
@@ -2016,9 +2152,10 @@
         <v>47</v>
       </c>
       <c r="F40" s="10"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
       <c r="B41" s="8" t="s">
         <v>14</v>
       </c>
@@ -2028,9 +2165,10 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="10"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
       <c r="B42" s="8" t="s">
         <v>16</v>
       </c>
@@ -2040,13 +2178,14 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="G42" s="24"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>10</v>
@@ -2056,11 +2195,12 @@
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="10"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="G44" s="24"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
       <c r="B45" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>10</v>
@@ -2069,12 +2209,13 @@
         <v>32</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="22"/>
       <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
@@ -2088,9 +2229,10 @@
         <v>47</v>
       </c>
       <c r="F46" s="10"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="22"/>
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -2100,9 +2242,10 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
+      <c r="G47" s="24"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
       <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
@@ -2112,13 +2255,18 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
+      <c r="G48" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A2:A26"/>
     <mergeCell ref="A29:A36"/>
     <mergeCell ref="A38:A42"/>
     <mergeCell ref="A44:A48"/>
+    <mergeCell ref="G2:G26"/>
+    <mergeCell ref="G29:G36"/>
+    <mergeCell ref="G38:G42"/>
+    <mergeCell ref="G44:G48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2126,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3ACC7-C065-475E-9BD1-DEB1E2424B3A}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2142,32 +2290,32 @@
     <col min="6" max="6" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>10</v>
@@ -2176,12 +2324,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="12"/>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
       <c r="B3" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>10</v>
@@ -2190,14 +2339,15 @@
         <v>32</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+        <v>106</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="24"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
       <c r="B4" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>10</v>
@@ -2208,14 +2358,15 @@
       <c r="E4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="F4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
       <c r="B5" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
@@ -2226,108 +2377,117 @@
       <c r="E5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="8" t="s">
-        <v>122</v>
+      <c r="F6" s="13"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
       <c r="B8" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
       <c r="B9" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
       <c r="B11" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
       <c r="B12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
       <c r="B13" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
@@ -2336,10 +2496,11 @@
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
@@ -2348,11 +2509,13 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A15"/>
+    <mergeCell ref="G2:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Severity Master table incorporated in DB Design for persisting Severity information.
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF0A628-C529-439C-8B1F-584755CA0146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC43367-EBB4-4A54-8FE3-4072B156FE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="129">
   <si>
     <t>Created By</t>
   </si>
@@ -405,6 +405,24 @@
   </si>
   <si>
     <t>USER_IS_PREGNANT</t>
+  </si>
+  <si>
+    <t>SEVERITY_MASTER</t>
+  </si>
+  <si>
+    <t>SEV_ID</t>
+  </si>
+  <si>
+    <t>SEV_NAME</t>
+  </si>
+  <si>
+    <t>ADEV_SEV_ID</t>
+  </si>
+  <si>
+    <t>REFERENCE TO SEV_ID OF SEVERITY_MASTER TABLE</t>
+  </si>
+  <si>
+    <t>This will be NULL for the Adverse Events whose IS_PARENT_ELEMENT is TRUE</t>
   </si>
 </sst>
 </file>
@@ -539,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,7 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -948,10 +965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4501CC-882B-43D3-A85F-1FC8AD5DCF77}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B48"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +1002,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -999,10 +1016,10 @@
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="24"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
@@ -1012,10 +1029,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="24"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1025,10 +1042,10 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="24"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1038,10 +1055,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1051,10 +1068,10 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1064,10 +1081,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>89</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1081,10 +1098,10 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1098,10 +1115,10 @@
         <v>94</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="8" t="s">
         <v>91</v>
       </c>
@@ -1111,10 +1128,10 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="8" t="s">
         <v>92</v>
       </c>
@@ -1124,10 +1141,10 @@
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="8" t="s">
         <v>93</v>
       </c>
@@ -1137,10 +1154,10 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1150,10 +1167,10 @@
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
@@ -1163,10 +1180,10 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="24"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="G15" s="23"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1180,10 +1197,10 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
@@ -1193,10 +1210,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="24"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="G18" s="23"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
@@ -1206,10 +1223,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
       <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1219,10 +1236,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="24"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="G20" s="23"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
       <c r="B21" s="8" t="s">
         <v>16</v>
       </c>
@@ -1232,14 +1249,14 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>59</v>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>123</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>10</v>
@@ -1249,12 +1266,12 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="24"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
       <c r="B24" s="8" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
@@ -1262,38 +1279,38 @@
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="24"/>
-    </row>
-    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="G24" s="23"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
       <c r="B25" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="24"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="23"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
       <c r="B26" s="8" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="24"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G26" s="23"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>15</v>
@@ -1301,69 +1318,55 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="24"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="24"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>63</v>
-      </c>
+      <c r="G27" s="23"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="23"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
       <c r="B30" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D30" s="8"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-    </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="23"/>
+    </row>
+    <row r="31" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
       <c r="B31" s="8" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-    </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+        <v>23</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="23"/>
+    </row>
+    <row r="32" spans="1:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
       <c r="B32" s="8" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>10</v>
@@ -1372,38 +1375,30 @@
         <v>32</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+        <v>128</v>
+      </c>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="8" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>15</v>
@@ -1411,72 +1406,92 @@
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="G34" s="23"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="23"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="8"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="24"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+      <c r="H37" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+    </row>
+    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
       <c r="B38" s="8" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="9"/>
       <c r="G38" s="24"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+    </row>
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
       <c r="B39" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="24"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="24"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>15</v>
@@ -1485,80 +1500,88 @@
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
       <c r="G40" s="24"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="8" t="s">
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="24"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="E43" s="9"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="23"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="24"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="24"/>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="24"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="23"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="8" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
       <c r="B47" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>15</v>
@@ -1566,38 +1589,122 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="24"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="8" t="s">
+      <c r="G47" s="23"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="23"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="23"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="23"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="23"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="23"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="23"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="22"/>
+      <c r="B55" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="24"/>
+      <c r="C55" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="H30:K34"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A42:A48"/>
+  <mergeCells count="17">
+    <mergeCell ref="G23:G27"/>
+    <mergeCell ref="H37:K41"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A49:A55"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A37:A41"/>
     <mergeCell ref="G2:G7"/>
     <mergeCell ref="G9:G15"/>
     <mergeCell ref="G17:G21"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="G42:G48"/>
-    <mergeCell ref="G30:G34"/>
+    <mergeCell ref="G29:G35"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="G49:G55"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1643,7 +1750,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1657,10 +1764,10 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="24"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1670,10 +1777,10 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="24"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
@@ -1687,10 +1794,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="24"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
@@ -1700,10 +1807,10 @@
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
@@ -1713,10 +1820,10 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
@@ -1726,10 +1833,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
@@ -1739,10 +1846,10 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
@@ -1752,10 +1859,10 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
@@ -1765,10 +1872,10 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
@@ -1778,10 +1885,10 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
@@ -1791,10 +1898,10 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="11" t="s">
         <v>72</v>
       </c>
@@ -1804,10 +1911,10 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="11" t="s">
         <v>70</v>
       </c>
@@ -1819,10 +1926,10 @@
         <v>71</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="11" t="s">
         <v>122</v>
       </c>
@@ -1832,10 +1939,10 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="11" t="s">
         <v>55</v>
       </c>
@@ -1847,10 +1954,10 @@
         <v>57</v>
       </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="11" t="s">
         <v>95</v>
       </c>
@@ -1864,10 +1971,10 @@
         <v>37</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="11" t="s">
         <v>96</v>
       </c>
@@ -1877,10 +1984,10 @@
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="24"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="11" t="s">
         <v>97</v>
       </c>
@@ -1890,10 +1997,10 @@
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="11" t="s">
         <v>98</v>
       </c>
@@ -1903,10 +2010,10 @@
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="24"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="11" t="s">
         <v>99</v>
       </c>
@@ -1916,10 +2023,10 @@
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="24"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="11" t="s">
         <v>100</v>
       </c>
@@ -1929,10 +2036,10 @@
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="24"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="11" t="s">
         <v>101</v>
       </c>
@@ -1942,10 +2049,10 @@
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="24"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="11" t="s">
         <v>50</v>
       </c>
@@ -1955,10 +2062,10 @@
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="24"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="11" t="s">
         <v>14</v>
       </c>
@@ -1968,10 +2075,10 @@
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
@@ -1981,10 +2088,10 @@
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="24"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1998,10 +2105,10 @@
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="24"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="11" t="s">
         <v>46</v>
       </c>
@@ -2015,10 +2122,10 @@
         <v>47</v>
       </c>
       <c r="F30" s="12"/>
-      <c r="G30" s="24"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="11" t="s">
         <v>48</v>
       </c>
@@ -2032,10 +2139,10 @@
         <v>49</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="G31" s="24"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="8" t="s">
         <v>102</v>
       </c>
@@ -2049,10 +2156,10 @@
         <v>103</v>
       </c>
       <c r="F32" s="13"/>
-      <c r="G32" s="24"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="11" t="s">
         <v>53</v>
       </c>
@@ -2062,10 +2169,10 @@
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="24"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="11" t="s">
         <v>51</v>
       </c>
@@ -2075,10 +2182,10 @@
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="24"/>
+      <c r="G34" s="23"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="11" t="s">
         <v>14</v>
       </c>
@@ -2088,10 +2195,10 @@
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="24"/>
+      <c r="G35" s="23"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="11" t="s">
         <v>16</v>
       </c>
@@ -2101,10 +2208,10 @@
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="24"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B38" s="8" t="s">
@@ -2118,10 +2225,10 @@
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="24"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="8" t="s">
         <v>74</v>
       </c>
@@ -2135,10 +2242,10 @@
         <v>85</v>
       </c>
       <c r="F39" s="9"/>
-      <c r="G39" s="24"/>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
       </c>
@@ -2152,10 +2259,10 @@
         <v>47</v>
       </c>
       <c r="F40" s="10"/>
-      <c r="G40" s="24"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="8" t="s">
         <v>14</v>
       </c>
@@ -2165,10 +2272,10 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="24"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="8" t="s">
         <v>16</v>
       </c>
@@ -2178,10 +2285,10 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="24"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="20" t="s">
         <v>86</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -2195,10 +2302,10 @@
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="24"/>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="8" t="s">
         <v>78</v>
       </c>
@@ -2212,10 +2319,10 @@
         <v>88</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="24"/>
+      <c r="G45" s="23"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
@@ -2229,10 +2336,10 @@
         <v>47</v>
       </c>
       <c r="F46" s="10"/>
-      <c r="G46" s="24"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -2242,10 +2349,10 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="24"/>
+      <c r="G47" s="23"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
@@ -2255,7 +2362,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
-      <c r="G48" s="24"/>
+      <c r="G48" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2276,8 +2383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3ACC7-C065-475E-9BD1-DEB1E2424B3A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,27 +2398,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -2325,10 +2432,10 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="24"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="11" t="s">
         <v>112</v>
       </c>
@@ -2342,10 +2449,10 @@
         <v>106</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="24"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="11" t="s">
         <v>111</v>
       </c>
@@ -2361,10 +2468,10 @@
       <c r="F4" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="11" t="s">
         <v>113</v>
       </c>
@@ -2380,11 +2487,11 @@
       <c r="F5" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="29" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="28" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -2393,10 +2500,10 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="11" t="s">
         <v>121</v>
       </c>
@@ -2406,10 +2513,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="11" t="s">
         <v>115</v>
       </c>
@@ -2419,10 +2526,10 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="11" t="s">
         <v>116</v>
       </c>
@@ -2432,10 +2539,10 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="11" t="s">
         <v>117</v>
       </c>
@@ -2445,10 +2552,10 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="11" t="s">
         <v>118</v>
       </c>
@@ -2458,10 +2565,10 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="11" t="s">
         <v>119</v>
       </c>
@@ -2471,10 +2578,10 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="11" t="s">
         <v>120</v>
       </c>
@@ -2484,10 +2591,10 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
@@ -2497,10 +2604,10 @@
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
@@ -2510,7 +2617,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Committed Rest Endpoint for getting the child Adverse Events
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF0C965-B70A-4EA8-ACC6-9CDAC3AB7278}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E34D66-6E33-4540-AEEE-9754F7A18804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
   <si>
     <t>Created By</t>
   </si>
@@ -426,6 +426,18 @@
   </si>
   <si>
     <t>SEV_ISACTIVE</t>
+  </si>
+  <si>
+    <t>Zafeer</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Rudra</t>
+  </si>
+  <si>
+    <t>Subhasis</t>
   </si>
 </sst>
 </file>
@@ -560,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,6 +649,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -970,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4501CC-882B-43D3-A85F-1FC8AD5DCF77}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +999,7 @@
     <col min="6" max="6" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>17</v>
       </c>
@@ -1020,8 +1035,12 @@
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
       <c r="G2" s="23"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="29"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
@@ -1033,8 +1052,10 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="23"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="8" t="s">
         <v>20</v>
@@ -1046,8 +1067,10 @@
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
       <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="8" t="s">
         <v>22</v>
@@ -1059,8 +1082,10 @@
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="23"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
@@ -1072,8 +1097,10 @@
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
       <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
@@ -1085,8 +1112,10 @@
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="23"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>89</v>
       </c>
@@ -1102,8 +1131,12 @@
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
       <c r="G9" s="23"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="8" t="s">
         <v>18</v>
@@ -1119,8 +1152,10 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="23"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="8" t="s">
         <v>91</v>
@@ -1132,8 +1167,10 @@
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
       <c r="G11" s="23"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="8" t="s">
         <v>92</v>
@@ -1145,8 +1182,10 @@
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="8" t="s">
         <v>93</v>
@@ -1158,8 +1197,10 @@
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
       <c r="G13" s="23"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
@@ -1171,8 +1212,10 @@
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
       <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
@@ -1184,8 +1227,10 @@
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
       <c r="G15" s="23"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>33</v>
       </c>
@@ -1201,8 +1246,12 @@
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
       <c r="G17" s="23"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="29"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
@@ -1214,8 +1263,10 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="23"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="8" t="s">
         <v>36</v>
@@ -1227,8 +1278,10 @@
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
       <c r="G19" s="23"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="8" t="s">
         <v>14</v>
@@ -1240,8 +1293,10 @@
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
       <c r="G20" s="23"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="8" t="s">
         <v>16</v>
@@ -1253,8 +1308,10 @@
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
       <c r="G21" s="23"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>123</v>
       </c>
@@ -1270,8 +1327,12 @@
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="23"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" s="29"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="8" t="s">
         <v>125</v>
@@ -1283,8 +1344,10 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="23"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="8" t="s">
         <v>129</v>
@@ -1296,8 +1359,10 @@
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="23"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="8" t="s">
         <v>14</v>
@@ -1309,8 +1374,10 @@
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
       <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="8" t="s">
         <v>16</v>
@@ -1322,8 +1389,10 @@
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
       <c r="G27" s="23"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>59</v>
       </c>
@@ -1339,8 +1408,12 @@
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
       <c r="G29" s="23"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I29" s="29"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="8" t="s">
         <v>61</v>
@@ -1352,8 +1425,10 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="23"/>
-    </row>
-    <row r="31" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+    </row>
+    <row r="31" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="8" t="s">
         <v>107</v>
@@ -1365,8 +1440,10 @@
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="23"/>
-    </row>
-    <row r="32" spans="1:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+    </row>
+    <row r="32" spans="1:9" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="8" t="s">
         <v>126</v>
@@ -1384,6 +1461,8 @@
         <v>128</v>
       </c>
       <c r="G32" s="23"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
@@ -1397,6 +1476,8 @@
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
       <c r="G33" s="23"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
@@ -1410,6 +1491,8 @@
       <c r="E34" s="9"/>
       <c r="F34" s="10"/>
       <c r="G34" s="23"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
@@ -1423,6 +1506,8 @@
       <c r="E35" s="9"/>
       <c r="F35" s="10"/>
       <c r="G35" s="23"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1541,6 +1626,10 @@
       <c r="E43" s="9"/>
       <c r="F43" s="10"/>
       <c r="G43" s="23"/>
+      <c r="H43" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
@@ -1554,6 +1643,8 @@
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="23"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
@@ -1567,6 +1658,8 @@
       <c r="E45" s="9"/>
       <c r="F45" s="10"/>
       <c r="G45" s="23"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
@@ -1580,6 +1673,8 @@
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
       <c r="G46" s="23"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
@@ -1593,8 +1688,10 @@
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
       <c r="G47" s="23"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>77</v>
       </c>
@@ -1610,8 +1707,12 @@
       <c r="E49" s="9"/>
       <c r="F49" s="10"/>
       <c r="G49" s="23"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="I49" s="29"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="8" t="s">
         <v>79</v>
@@ -1623,8 +1724,10 @@
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="23"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="8" t="s">
         <v>81</v>
@@ -1636,8 +1739,10 @@
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="23"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="8" t="s">
         <v>82</v>
@@ -1649,8 +1754,10 @@
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="23"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="8" t="s">
         <v>80</v>
@@ -1662,8 +1769,10 @@
       <c r="E53" s="9"/>
       <c r="F53" s="10"/>
       <c r="G53" s="23"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="8" t="s">
         <v>14</v>
@@ -1675,8 +1784,10 @@
       <c r="E54" s="9"/>
       <c r="F54" s="10"/>
       <c r="G54" s="23"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
       <c r="B55" s="8" t="s">
         <v>16</v>
@@ -1688,10 +1799,19 @@
       <c r="E55" s="9"/>
       <c r="F55" s="10"/>
       <c r="G55" s="23"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="24">
+    <mergeCell ref="H49:I55"/>
     <mergeCell ref="G23:G27"/>
+    <mergeCell ref="H43:I47"/>
+    <mergeCell ref="H2:I7"/>
+    <mergeCell ref="H9:I15"/>
+    <mergeCell ref="H17:I21"/>
+    <mergeCell ref="H23:I27"/>
+    <mergeCell ref="H29:I35"/>
     <mergeCell ref="H37:K41"/>
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A49:A55"/>
@@ -2387,7 +2507,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the entities and repositories related to the DB Structural changes and some other changes.
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E34D66-6E33-4540-AEEE-9754F7A18804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A637DF-3023-407B-BA2A-25ED77A65FEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="122">
   <si>
     <t>Created By</t>
   </si>
@@ -227,27 +227,9 @@
     <t>ADEV_ISACTIVE</t>
   </si>
   <si>
-    <t>ADVERSE_EVENT_MAPPING</t>
-  </si>
-  <si>
-    <t>ADEV_MAPPING_ID</t>
-  </si>
-  <si>
-    <t>ADEV_MAPPING_ADEV_ID</t>
-  </si>
-  <si>
     <t>REFERENCE TO ADEV_ID OF ADVERSE_EVENT_MASTER TABLE</t>
   </si>
   <si>
-    <t>ADEV_MAPPING_PARENT_ADEV_ID</t>
-  </si>
-  <si>
-    <t>This will be NULL for the Adverse Events falling at the root level of classification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There will be multiple entries for each Adverse Event in this table since the underlying adverse events can be same for two Root level adverse events. For example, Head-ache is common for Fever and Vomiting </t>
-  </si>
-  <si>
     <t>USER_SEX</t>
   </si>
   <si>
@@ -359,27 +341,12 @@
     <t>REFERENCE TO USVAC_ID OF USER_VACCINE TABLE</t>
   </si>
   <si>
-    <t>ADEV_IS_PARENT_ELEMENT</t>
-  </si>
-  <si>
-    <t>This should contain the ID of the Adverse_Event_Master entries in which the ADEV_IS_PARENT_ELEMENT is TRUE</t>
-  </si>
-  <si>
-    <t>This should contain the ID of the Adverse_Event_Master entries in which the ADEV_IS_PARENT_ELEMENT is FALSE</t>
-  </si>
-  <si>
     <t>CLOB</t>
   </si>
   <si>
-    <t>ADEV_REP_PARENT_ADEV_ID</t>
-  </si>
-  <si>
     <t>ADEV_REP_USVAC_ID</t>
   </si>
   <si>
-    <t>ADEV_REP_CHILD_ADEV_ID</t>
-  </si>
-  <si>
     <t>ADEV_REP_ADDITIONAL_NOTES</t>
   </si>
   <si>
@@ -416,15 +383,9 @@
     <t>SEV_NAME</t>
   </si>
   <si>
-    <t>ADEV_SEV_ID</t>
-  </si>
-  <si>
     <t>REFERENCE TO SEV_ID OF SEVERITY_MASTER TABLE</t>
   </si>
   <si>
-    <t>This will be NULL for the Adverse Events whose IS_PARENT_ELEMENT is TRUE</t>
-  </si>
-  <si>
     <t>SEV_ISACTIVE</t>
   </si>
   <si>
@@ -434,17 +395,20 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Rudra</t>
-  </si>
-  <si>
     <t>Subhasis</t>
+  </si>
+  <si>
+    <t>ADEV_REP_ADEV_ID</t>
+  </si>
+  <si>
+    <t>ADEV_REP_SEV_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,12 +420,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -572,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -607,10 +565,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,9 +573,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -635,9 +586,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -646,9 +594,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -983,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4501CC-882B-43D3-A85F-1FC8AD5DCF77}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +965,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1034,14 +979,14 @@
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="29"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
@@ -1051,12 +996,12 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1066,12 +1011,12 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1081,12 +1026,12 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1096,12 +1041,12 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1111,16 +1056,16 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>89</v>
+      <c r="A9" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -1130,14 +1075,14 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="I9" s="29"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1148,17 +1093,17 @@
         <v>32</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>13</v>
@@ -1166,14 +1111,14 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>52</v>
@@ -1181,14 +1126,14 @@
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>23</v>
@@ -1196,12 +1141,12 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1211,12 +1156,12 @@
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
@@ -1226,12 +1171,12 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1245,14 +1190,14 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="I17" s="29"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
@@ -1262,12 +1207,12 @@
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
@@ -1277,12 +1222,12 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1292,12 +1237,12 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="8" t="s">
         <v>16</v>
       </c>
@@ -1307,16 +1252,16 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>123</v>
+      <c r="A23" s="17" t="s">
+        <v>112</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>10</v>
@@ -1326,16 +1271,16 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="I23" s="29"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" s="24"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="8" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
@@ -1343,14 +1288,14 @@
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="8" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>23</v>
@@ -1358,12 +1303,12 @@
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="8" t="s">
         <v>14</v>
       </c>
@@ -1373,12 +1318,12 @@
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="8" t="s">
         <v>16</v>
       </c>
@@ -1388,12 +1333,12 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="8" t="s">
@@ -1407,14 +1352,14 @@
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="I29" s="29"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="8" t="s">
         <v>61</v>
       </c>
@@ -1424,162 +1369,125 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-    </row>
-    <row r="31" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
       <c r="B31" s="8" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-    </row>
-    <row r="32" spans="1:9" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
       <c r="B32" s="8" t="s">
-        <v>126</v>
+        <v>14</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+        <v>15</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
       <c r="B33" s="8" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="8" t="s">
+      <c r="G33" s="20"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I36" s="24"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="8" t="s">
+      <c r="C39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
+      <c r="B40" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-    </row>
-    <row r="38" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-    </row>
-    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" s="24"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>15</v>
@@ -1587,67 +1495,63 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+      <c r="G40" s="20"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I42" s="24"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="I43" s="29"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
       <c r="B44" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
       <c r="B45" s="8" t="s">
         <v>76</v>
       </c>
@@ -1656,30 +1560,30 @@
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
       <c r="B46" s="8" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
       <c r="B47" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>15</v>
@@ -1687,146 +1591,47 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="I49" s="29"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
-      <c r="B53" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
-      <c r="B54" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="8" t="s">
+      <c r="G47" s="20"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
+      <c r="C48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="H49:I55"/>
+  <mergeCells count="21">
+    <mergeCell ref="H42:I48"/>
     <mergeCell ref="G23:G27"/>
-    <mergeCell ref="H43:I47"/>
+    <mergeCell ref="H36:I40"/>
     <mergeCell ref="H2:I7"/>
     <mergeCell ref="H9:I15"/>
     <mergeCell ref="H17:I21"/>
     <mergeCell ref="H23:I27"/>
-    <mergeCell ref="H29:I35"/>
-    <mergeCell ref="H37:K41"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="H29:I33"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A42:A48"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A29:A33"/>
     <mergeCell ref="G2:G7"/>
     <mergeCell ref="G9:G15"/>
     <mergeCell ref="G17:G21"/>
-    <mergeCell ref="G29:G35"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="G49:G55"/>
-    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G42:G48"/>
     <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1838,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F028140-CA34-4194-A102-025CA8E62727}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1678,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1887,10 +1692,10 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="23"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1900,10 +1705,10 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="23"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
@@ -1917,10 +1722,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="23"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
@@ -1930,10 +1735,10 @@
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="23"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
@@ -1943,10 +1748,10 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
@@ -1956,10 +1761,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
@@ -1969,10 +1774,10 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
@@ -1982,10 +1787,10 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
@@ -1995,10 +1800,10 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
@@ -2008,10 +1813,10 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
@@ -2021,12 +1826,12 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>15</v>
@@ -2034,27 +1839,27 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="11" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>23</v>
@@ -2062,10 +1867,10 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="11" t="s">
         <v>55</v>
       </c>
@@ -2077,12 +1882,12 @@
         <v>57</v>
       </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>10</v>
@@ -2094,12 +1899,12 @@
         <v>37</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>13</v>
@@ -2107,12 +1912,12 @@
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="23"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>13</v>
@@ -2120,12 +1925,12 @@
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="23"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>13</v>
@@ -2133,12 +1938,12 @@
       <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>39</v>
@@ -2146,12 +1951,12 @@
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="23"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>39</v>
@@ -2159,12 +1964,12 @@
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>13</v>
@@ -2172,10 +1977,10 @@
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="11" t="s">
         <v>50</v>
       </c>
@@ -2185,10 +1990,10 @@
       <c r="D24" s="11"/>
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="23"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="11" t="s">
         <v>14</v>
       </c>
@@ -2198,10 +2003,10 @@
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="23"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
@@ -2211,10 +2016,10 @@
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="21" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -2228,10 +2033,10 @@
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="23"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="11" t="s">
         <v>46</v>
       </c>
@@ -2245,10 +2050,10 @@
         <v>47</v>
       </c>
       <c r="F30" s="12"/>
-      <c r="G30" s="23"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="11" t="s">
         <v>48</v>
       </c>
@@ -2262,12 +2067,12 @@
         <v>49</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="G31" s="23"/>
+      <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>10</v>
@@ -2276,13 +2081,13 @@
         <v>32</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F32" s="13"/>
-      <c r="G32" s="23"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="11" t="s">
         <v>53</v>
       </c>
@@ -2292,10 +2097,10 @@
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="23"/>
+      <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="11" t="s">
         <v>51</v>
       </c>
@@ -2305,10 +2110,10 @@
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="23"/>
+      <c r="G34" s="20"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="11" t="s">
         <v>14</v>
       </c>
@@ -2318,10 +2123,10 @@
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="23"/>
+      <c r="G35" s="20"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="11" t="s">
         <v>16</v>
       </c>
@@ -2331,14 +2136,14 @@
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
-      <c r="G36" s="23"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>83</v>
+      <c r="A38" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>10</v>
@@ -2348,12 +2153,12 @@
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="23"/>
+      <c r="G38" s="20"/>
     </row>
     <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>10</v>
@@ -2362,13 +2167,13 @@
         <v>32</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F39" s="9"/>
-      <c r="G39" s="23"/>
+      <c r="G39" s="20"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="8" t="s">
         <v>25</v>
       </c>
@@ -2382,10 +2187,10 @@
         <v>47</v>
       </c>
       <c r="F40" s="10"/>
-      <c r="G40" s="23"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="8" t="s">
         <v>14</v>
       </c>
@@ -2395,10 +2200,10 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="23"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="8" t="s">
         <v>16</v>
       </c>
@@ -2408,14 +2213,14 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="23"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>86</v>
+      <c r="A44" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>10</v>
@@ -2425,12 +2230,12 @@
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="23"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>10</v>
@@ -2439,13 +2244,13 @@
         <v>32</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="23"/>
+      <c r="G45" s="20"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
@@ -2459,10 +2264,10 @@
         <v>47</v>
       </c>
       <c r="F46" s="10"/>
-      <c r="G46" s="23"/>
+      <c r="G46" s="20"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -2472,10 +2277,10 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="23"/>
+      <c r="G47" s="20"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
@@ -2485,7 +2290,7 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
-      <c r="G48" s="23"/>
+      <c r="G48" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2506,8 +2311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3ACC7-C065-475E-9BD1-DEB1E2424B3A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,31 +2326,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>104</v>
+      <c r="A2" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>10</v>
@@ -2555,12 +2360,12 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="23"/>
+      <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="11" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>10</v>
@@ -2569,15 +2374,15 @@
         <v>32</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="23"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="11" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>10</v>
@@ -2586,17 +2391,15 @@
         <v>32</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+        <v>63</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
       <c r="B5" s="11" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
@@ -2605,30 +2408,28 @@
         <v>32</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G5" s="23"/>
+        <v>115</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="28" t="s">
-        <v>114</v>
+      <c r="A6" s="22"/>
+      <c r="B6" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="11" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>54</v>
@@ -2636,12 +2437,12 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="23"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="11" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>23</v>
@@ -2649,12 +2450,12 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="23"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="11" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>15</v>
@@ -2662,12 +2463,12 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="23"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="11" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -2675,25 +2476,25 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="11" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="11" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>23</v>
@@ -2701,12 +2502,12 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="11" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>15</v>
@@ -2714,10 +2515,10 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="23"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
@@ -2727,10 +2528,10 @@
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
@@ -2740,7 +2541,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="23"/>
+      <c r="G15" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Commit for Adverse Event Reporting, Email, OTP and DB Document.
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A637DF-3023-407B-BA2A-25ED77A65FEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33CD405-6CFD-44B9-AEB9-5D6BF77F79FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Info" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Adverse Event Tables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="142">
   <si>
     <t>Created By</t>
   </si>
@@ -203,9 +204,6 @@
     <t>TIMESTAMP</t>
   </si>
   <si>
-    <t>USER_INFO_ADDED_BY</t>
-  </si>
-  <si>
     <t>ENUMERATION</t>
   </si>
   <si>
@@ -305,27 +303,6 @@
     <t>REFERENCE TOVACCINE_ID OF VACCINE_MASTER TABLE</t>
   </si>
   <si>
-    <t>USER_REPORTER_TITLE_ID</t>
-  </si>
-  <si>
-    <t>USER_REPORTER_FIRST_NAME</t>
-  </si>
-  <si>
-    <t>USER_REPORTER_MIDDLE_NAME</t>
-  </si>
-  <si>
-    <t>USER_REPORTER_LAST_NAME</t>
-  </si>
-  <si>
-    <t>USER_REPORTER_MOBILE_NUMBER</t>
-  </si>
-  <si>
-    <t>USER_REPORTER_ALTERNATE_NUMBER</t>
-  </si>
-  <si>
-    <t>USER_REPORTER_EMAIL_ID</t>
-  </si>
-  <si>
     <t>USVAC_VACCINE_DOSE_ID</t>
   </si>
   <si>
@@ -402,6 +379,90 @@
   </si>
   <si>
     <t>ADEV_REP_SEV_ID</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_ID</t>
+  </si>
+  <si>
+    <t>VARCHAR (15)</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_USER_ID</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_ CASE_ID</t>
+  </si>
+  <si>
+    <t>CASE_INFO_ADDED_BY</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_TITLE_ID</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_FIRST_NAME</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_MIDDLE_NAME</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_LAST_NAME</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_MOBILE_NUMBER</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_ALTERNATE_NUMBER</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_EMAIL_ID</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER</t>
+  </si>
+  <si>
+    <t>OTP_ID</t>
+  </si>
+  <si>
+    <t>OTP_CODES</t>
+  </si>
+  <si>
+    <t>OTP_VALUE</t>
+  </si>
+  <si>
+    <t>VARCHAR(5)</t>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>OTP_ACTIVE</t>
+  </si>
+  <si>
+    <t>OTP_EMAIL_ID</t>
+  </si>
+  <si>
+    <t>MD_ID</t>
+  </si>
+  <si>
+    <t>OTP, REPORTING</t>
+  </si>
+  <si>
+    <t>MD_CODE</t>
+  </si>
+  <si>
+    <t>MD_SUBJECT</t>
+  </si>
+  <si>
+    <t>MD_BODY</t>
+  </si>
+  <si>
+    <t>MAIL_DETAIL</t>
+  </si>
+  <si>
+    <t>MD_FROM_EMAIL</t>
+  </si>
+  <si>
+    <t>MD_FROM_EMAIL_NAME</t>
   </si>
 </sst>
 </file>
@@ -530,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -583,6 +644,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -595,7 +659,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,11 +1043,11 @@
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="24"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
@@ -996,9 +1060,9 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
@@ -1011,9 +1075,9 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -1026,9 +1090,9 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
@@ -1041,9 +1105,9 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -1056,16 +1120,16 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
@@ -1075,11 +1139,11 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="24"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
@@ -1093,17 +1157,17 @@
         <v>32</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>13</v>
@@ -1111,14 +1175,14 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>52</v>
@@ -1126,14 +1190,14 @@
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>23</v>
@@ -1141,9 +1205,9 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
@@ -1156,9 +1220,9 @@
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
@@ -1171,9 +1235,9 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
@@ -1190,11 +1254,11 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" s="24"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
@@ -1207,9 +1271,9 @@
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -1222,9 +1286,9 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -1237,9 +1301,9 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
@@ -1252,16 +1316,16 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>10</v>
@@ -1271,16 +1335,16 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I23" s="24"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>13</v>
@@ -1288,14 +1352,14 @@
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>23</v>
@@ -1303,9 +1367,9 @@
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
@@ -1318,9 +1382,9 @@
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
@@ -1333,16 +1397,16 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>10</v>
@@ -1352,16 +1416,16 @@
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="I29" s="24"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>13</v>
@@ -1369,14 +1433,14 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>23</v>
@@ -1384,9 +1448,9 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
@@ -1399,9 +1463,9 @@
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
@@ -1414,16 +1478,16 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>10</v>
@@ -1433,16 +1497,16 @@
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" s="24"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I36" s="20"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>35</v>
@@ -1450,14 +1514,14 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>23</v>
@@ -1465,9 +1529,9 @@
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
@@ -1480,9 +1544,9 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
@@ -1495,16 +1559,16 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>10</v>
@@ -1514,16 +1578,16 @@
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I42" s="24"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I42" s="20"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>35</v>
@@ -1531,14 +1595,14 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>23</v>
@@ -1546,14 +1610,14 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>23</v>
@@ -1561,14 +1625,14 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>23</v>
@@ -1576,9 +1640,9 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
@@ -1591,9 +1655,9 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
@@ -1606,9 +1670,9 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -1620,18 +1684,18 @@
     <mergeCell ref="H17:I21"/>
     <mergeCell ref="H23:I27"/>
     <mergeCell ref="H29:I33"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G9:G15"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G42:G48"/>
     <mergeCell ref="A36:A40"/>
     <mergeCell ref="A42:A48"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A29:A33"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="G9:G15"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="G42:G48"/>
     <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1641,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F028140-CA34-4194-A102-025CA8E62727}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,7 +1742,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1692,10 +1756,10 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="20"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1705,10 +1769,10 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
@@ -1722,10 +1786,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="20"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
@@ -1735,10 +1799,10 @@
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
@@ -1748,10 +1812,10 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
@@ -1761,10 +1825,10 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="11" t="s">
         <v>38</v>
       </c>
@@ -1774,10 +1838,10 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="11" t="s">
         <v>40</v>
       </c>
@@ -1787,10 +1851,10 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
@@ -1800,10 +1864,10 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="11" t="s">
         <v>42</v>
       </c>
@@ -1813,12 +1877,12 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>10</v>
@@ -1826,12 +1890,12 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>15</v>
@@ -1839,27 +1903,27 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="13"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="11" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>23</v>
@@ -1867,375 +1931,392 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
       <c r="B17" s="11" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="20"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="25" t="s">
+        <v>126</v>
+      </c>
       <c r="B20" s="11" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="20"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="11" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="20"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
       <c r="B23" s="11" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
+      <c r="B24" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>13</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="20"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="20"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="11" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="20"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="21"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="21"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="25"/>
+      <c r="B29" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="13"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B34" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="C34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="11" t="s">
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="11" t="s">
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E35" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="20"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="10"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="21"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="21"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="C41" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="21"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="9"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C43" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="20"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="20"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="20"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="21"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="8" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>10</v>
@@ -2243,67 +2324,283 @@
       <c r="D45" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E45" s="12" t="s">
-        <v>82</v>
+      <c r="E45" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="20"/>
+      <c r="G45" s="21"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="20"/>
+        <v>14</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="20"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="8" t="s">
+      <c r="F47" s="9"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="19"/>
+      <c r="B53" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="20"/>
+      <c r="C53" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="12"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="9"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="8"/>
+      <c r="E60" s="9"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="9"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="11"/>
+      <c r="E63" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" s="11"/>
+      <c r="E64" s="12"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D65" s="11"/>
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="11"/>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" s="11"/>
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="9"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A2:A26"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="G2:G26"/>
-    <mergeCell ref="G29:G36"/>
-    <mergeCell ref="G38:G42"/>
-    <mergeCell ref="G44:G48"/>
+  <mergeCells count="11">
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A62:A69"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="G2:G18"/>
+    <mergeCell ref="G35:G39"/>
+    <mergeCell ref="G41:G45"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="G20:G33"/>
+    <mergeCell ref="A20:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2311,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF3ACC7-C065-475E-9BD1-DEB1E2424B3A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,11 +2643,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>98</v>
+      <c r="A2" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>10</v>
@@ -2360,12 +2657,12 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="20"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>10</v>
@@ -2374,15 +2671,15 @@
         <v>32</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="20"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="11" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>10</v>
@@ -2391,15 +2688,15 @@
         <v>32</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="20"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="11" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
@@ -2408,28 +2705,28 @@
         <v>32</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="11" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="11" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>54</v>
@@ -2437,12 +2734,12 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>23</v>
@@ -2450,12 +2747,12 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="11" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>15</v>
@@ -2463,12 +2760,12 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -2476,25 +2773,25 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="11" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>23</v>
@@ -2502,12 +2799,12 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>15</v>
@@ -2515,10 +2812,10 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
@@ -2528,10 +2825,10 @@
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
@@ -2541,7 +2838,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Changes related to the addition of the Beneficiary Reference ID
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33CD405-6CFD-44B9-AEB9-5D6BF77F79FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A60654-191C-4F67-94E1-3DCF076522E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="144">
   <si>
     <t>Created By</t>
   </si>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t>MD_FROM_EMAIL_NAME</t>
+  </si>
+  <si>
+    <t>USER_BENEFICIARY_REF_ID</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
   </si>
 </sst>
 </file>
@@ -1705,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F028140-CA34-4194-A102-025CA8E62727}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,40 +1777,40 @@
       <c r="F3" s="12"/>
       <c r="G3" s="21"/>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="12"/>
       <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>13</v>
@@ -1817,7 +1823,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>13</v>
@@ -1830,10 +1836,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
@@ -1843,7 +1849,7 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>39</v>
@@ -1856,10 +1862,10 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
@@ -1869,10 +1875,10 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
@@ -1882,10 +1888,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="11" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
@@ -1895,10 +1901,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
@@ -1908,51 +1914,51 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="12" t="s">
-        <v>64</v>
-      </c>
+      <c r="E14" s="12"/>
       <c r="F14" s="13"/>
       <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="11" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="F15" s="13"/>
       <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="11" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
@@ -1962,7 +1968,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>15</v>
@@ -1972,32 +1978,32 @@
       <c r="F18" s="12"/>
       <c r="G18" s="21"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="C21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="21"/>
@@ -2005,31 +2011,29 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>47</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="21"/>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="E23" s="12" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="21"/>
@@ -2037,37 +2041,39 @@
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>32</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="21"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="F25" s="12"/>
       <c r="G25" s="21"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>13</v>
@@ -2080,7 +2086,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>13</v>
@@ -2093,10 +2099,10 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
@@ -2106,7 +2112,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>39</v>
@@ -2119,10 +2125,10 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
@@ -2132,10 +2138,10 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="11" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
@@ -2145,7 +2151,7 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>15</v>
@@ -2156,45 +2162,41 @@
       <c r="G32" s="21"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F33" s="13"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
       <c r="G33" s="21"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="F34" s="13"/>
+      <c r="G34" s="21"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B35" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>10</v>
@@ -2203,15 +2205,15 @@
         <v>32</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="F36" s="10"/>
       <c r="G36" s="21"/>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
-      <c r="B37" s="8" t="s">
-        <v>88</v>
+      <c r="B37" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>10</v>
@@ -2220,31 +2222,35 @@
         <v>32</v>
       </c>
       <c r="E37" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="21"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
       <c r="F38" s="10"/>
       <c r="G38" s="21"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="12"/>
@@ -2254,69 +2260,65 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="11" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="12"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="12"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="9"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="10"/>
       <c r="G42" s="21"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="21"/>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="B44" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>78</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="21"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="8" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>10</v>
@@ -2325,7 +2327,7 @@
         <v>32</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="21"/>
@@ -2333,19 +2335,24 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>15</v>
@@ -2354,40 +2361,37 @@
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="C50" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="E50" s="9"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="8" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>10</v>
@@ -2396,24 +2400,28 @@
         <v>32</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
-      <c r="B53" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>15</v>
@@ -2421,39 +2429,39 @@
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+      <c r="B54" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B56" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="8" t="s">
+      <c r="C56" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="12"/>
+      <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
       <c r="B57" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="12"/>
@@ -2461,10 +2469,10 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
       <c r="B58" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="D58" s="11"/>
       <c r="E58" s="12"/>
@@ -2472,18 +2480,18 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
       <c r="B59" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D59" s="11"/>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="9"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
-      <c r="B60" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>15</v>
@@ -2491,49 +2499,49 @@
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="19"/>
+      <c r="B61" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="9"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B63" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62" s="8" t="s">
+      <c r="C63" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="9"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D63" s="11"/>
-      <c r="E63" s="12" t="s">
-        <v>135</v>
-      </c>
+      <c r="E63" s="9"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="18"/>
       <c r="B64" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="D64" s="11"/>
-      <c r="E64" s="12"/>
+      <c r="E64" s="12" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="18"/>
       <c r="B65" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>131</v>
@@ -2544,7 +2552,7 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="18"/>
       <c r="B66" s="8" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>131</v>
@@ -2555,7 +2563,7 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="18"/>
       <c r="B67" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>131</v>
@@ -2566,18 +2574,18 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="18"/>
       <c r="B68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" s="11"/>
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="9"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>15</v>
@@ -2585,19 +2593,30 @@
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="8"/>
+      <c r="E70" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A62:A69"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="G2:G18"/>
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="G41:G45"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="G20:G33"/>
-    <mergeCell ref="A20:A32"/>
+    <mergeCell ref="A56:A61"/>
+    <mergeCell ref="A63:A70"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="G21:G34"/>
+    <mergeCell ref="A21:A33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commit for Search functionality based on Aadhaar Card. Please refer to the mail for DB scripts and changes.
</commit_message>
<xml_diff>
--- a/Documents/CFC-VAERS-Database-Design.xlsx
+++ b/Documents/CFC-VAERS-Database-Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SUBHASIS\CFC\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A60654-191C-4F67-94E1-3DCF076522E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9FD6D2-531E-4F67-9A9F-675425C46042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="145">
   <si>
     <t>Created By</t>
   </si>
@@ -387,9 +387,6 @@
     <t>VARCHAR (15)</t>
   </si>
   <si>
-    <t>CASE_REPORTER_USER_ID</t>
-  </si>
-  <si>
     <t>CASE_REPORTER_ CASE_ID</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>MD_ID</t>
   </si>
   <si>
-    <t>OTP, REPORTING</t>
-  </si>
-  <si>
     <t>MD_CODE</t>
   </si>
   <si>
@@ -469,6 +463,15 @@
   </si>
   <si>
     <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>OTP, REPORTING, SEARCH</t>
+  </si>
+  <si>
+    <t>CASE_REPORTER_USVAC_ID</t>
+  </si>
+  <si>
+    <t>REFERENCE TO USER_ID OF USER_VACCINE TABLE</t>
   </si>
 </sst>
 </file>
@@ -641,6 +644,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -649,12 +658,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1035,7 +1038,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1049,14 +1052,14 @@
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="20"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
@@ -1066,12 +1069,12 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1081,12 +1084,12 @@
       <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
@@ -1096,12 +1099,12 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1111,12 +1114,12 @@
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1126,12 +1129,12 @@
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="19" t="s">
         <v>82</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1145,14 +1148,14 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="20" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1166,12 +1169,12 @@
         <v>87</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="8" t="s">
         <v>84</v>
       </c>
@@ -1181,12 +1184,12 @@
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="8" t="s">
         <v>85</v>
       </c>
@@ -1196,12 +1199,12 @@
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="8" t="s">
         <v>86</v>
       </c>
@@ -1211,12 +1214,12 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1226,12 +1229,12 @@
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
@@ -1241,12 +1244,12 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="19" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1260,14 +1263,14 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="20" t="s">
+      <c r="G17" s="18"/>
+      <c r="H17" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
@@ -1277,12 +1280,12 @@
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="8" t="s">
         <v>36</v>
       </c>
@@ -1292,12 +1295,12 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
@@ -1307,12 +1310,12 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="8" t="s">
         <v>16</v>
       </c>
@@ -1322,12 +1325,12 @@
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="19" t="s">
         <v>104</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1341,14 +1344,14 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="20" t="s">
+      <c r="G23" s="18"/>
+      <c r="H23" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="17"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="8" t="s">
         <v>106</v>
       </c>
@@ -1358,12 +1361,12 @@
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="8" t="s">
         <v>108</v>
       </c>
@@ -1373,12 +1376,12 @@
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="8" t="s">
         <v>14</v>
       </c>
@@ -1388,12 +1391,12 @@
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="8" t="s">
         <v>16</v>
       </c>
@@ -1403,12 +1406,12 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B29" s="8" t="s">
@@ -1422,14 +1425,14 @@
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="20" t="s">
+      <c r="G29" s="18"/>
+      <c r="H29" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="I29" s="20"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="8" t="s">
         <v>60</v>
       </c>
@@ -1439,12 +1442,12 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="8" t="s">
         <v>61</v>
       </c>
@@ -1454,12 +1457,12 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -1469,12 +1472,12 @@
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="8" t="s">
         <v>16</v>
       </c>
@@ -1484,12 +1487,12 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B36" s="8" t="s">
@@ -1503,14 +1506,14 @@
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="20" t="s">
+      <c r="G36" s="18"/>
+      <c r="H36" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="I36" s="20"/>
+      <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="8" t="s">
         <v>68</v>
       </c>
@@ -1520,12 +1523,12 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="8" t="s">
         <v>69</v>
       </c>
@@ -1535,12 +1538,12 @@
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="8" t="s">
         <v>14</v>
       </c>
@@ -1550,12 +1553,12 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="8" t="s">
         <v>16</v>
       </c>
@@ -1565,12 +1568,12 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="19" t="s">
         <v>70</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -1584,14 +1587,14 @@
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="20" t="s">
+      <c r="G42" s="18"/>
+      <c r="H42" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="I42" s="20"/>
+      <c r="I42" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="8" t="s">
         <v>72</v>
       </c>
@@ -1601,12 +1604,12 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="8" t="s">
         <v>74</v>
       </c>
@@ -1616,12 +1619,12 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="8" t="s">
         <v>75</v>
       </c>
@@ -1631,12 +1634,12 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="8" t="s">
         <v>73</v>
       </c>
@@ -1646,12 +1649,12 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -1661,12 +1664,12 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
@@ -1676,12 +1679,19 @@
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="10"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A23:A27"/>
     <mergeCell ref="H42:I48"/>
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="H36:I40"/>
@@ -1696,13 +1706,6 @@
     <mergeCell ref="G29:G33"/>
     <mergeCell ref="G36:G40"/>
     <mergeCell ref="G42:G48"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A23:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1714,7 +1717,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,7 +1765,7 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="21"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
@@ -1775,20 +1778,20 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="21"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="21"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
@@ -1805,7 +1808,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
@@ -1818,7 +1821,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
@@ -1831,7 +1834,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
@@ -1844,7 +1847,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
@@ -1857,7 +1860,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
@@ -1870,7 +1873,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
@@ -1883,7 +1886,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
@@ -1896,7 +1899,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
@@ -1909,7 +1912,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="21"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
@@ -1922,7 +1925,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
@@ -1937,7 +1940,7 @@
         <v>64</v>
       </c>
       <c r="F15" s="13"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
@@ -1950,7 +1953,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
@@ -1963,7 +1966,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
@@ -1976,7 +1979,7 @@
       <c r="D18" s="11"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="21"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
@@ -1989,11 +1992,11 @@
       <c r="D19" s="11"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>114</v>
@@ -2006,12 +2009,12 @@
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="21"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>115</v>
@@ -2019,12 +2022,12 @@
       <c r="D22" s="11"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="21"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="11" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>10</v>
@@ -2033,15 +2036,15 @@
         <v>32</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="21"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>55</v>
@@ -2051,12 +2054,12 @@
         <v>56</v>
       </c>
       <c r="F24" s="12"/>
-      <c r="G24" s="21"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>10</v>
@@ -2068,12 +2071,12 @@
         <v>37</v>
       </c>
       <c r="F25" s="12"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>13</v>
@@ -2081,12 +2084,12 @@
       <c r="D26" s="11"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="21"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>13</v>
@@ -2094,12 +2097,12 @@
       <c r="D27" s="11"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="21"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>13</v>
@@ -2107,12 +2110,12 @@
       <c r="D28" s="11"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
-      <c r="G28" s="21"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>39</v>
@@ -2120,12 +2123,12 @@
       <c r="D29" s="11"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="21"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>39</v>
@@ -2133,12 +2136,12 @@
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="21"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>13</v>
@@ -2146,7 +2149,7 @@
       <c r="D31" s="11"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="21"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
@@ -2159,7 +2162,7 @@
       <c r="D32" s="11"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
-      <c r="G32" s="21"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
@@ -2172,11 +2175,11 @@
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="21"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" s="13"/>
-      <c r="G34" s="21"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
@@ -2208,7 +2211,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="10"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
@@ -2225,7 +2228,7 @@
         <v>49</v>
       </c>
       <c r="F37" s="9"/>
-      <c r="G37" s="21"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
@@ -2242,7 +2245,7 @@
         <v>89</v>
       </c>
       <c r="F38" s="10"/>
-      <c r="G38" s="21"/>
+      <c r="G38" s="18"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
@@ -2255,7 +2258,7 @@
       <c r="D39" s="11"/>
       <c r="E39" s="12"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="21"/>
+      <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
@@ -2268,7 +2271,7 @@
       <c r="D40" s="11"/>
       <c r="E40" s="12"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="21"/>
+      <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
@@ -2292,14 +2295,14 @@
       <c r="D42" s="11"/>
       <c r="E42" s="12"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="21"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F43" s="9"/>
-      <c r="G43" s="21"/>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="19" t="s">
         <v>76</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -2313,10 +2316,10 @@
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="21"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="8" t="s">
         <v>67</v>
       </c>
@@ -2330,10 +2333,10 @@
         <v>78</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="21"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
+      <c r="A46" s="20"/>
       <c r="B46" s="8" t="s">
         <v>25</v>
       </c>
@@ -2347,10 +2350,10 @@
         <v>47</v>
       </c>
       <c r="F46" s="9"/>
-      <c r="G46" s="21"/>
+      <c r="G46" s="18"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -2362,7 +2365,7 @@
       <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="8" t="s">
         <v>16</v>
       </c>
@@ -2374,7 +2377,7 @@
       <c r="F48" s="9"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="19" t="s">
         <v>79</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -2389,7 +2392,7 @@
       <c r="E50" s="9"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
+      <c r="A51" s="20"/>
       <c r="B51" s="8" t="s">
         <v>71</v>
       </c>
@@ -2404,7 +2407,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
+      <c r="A52" s="20"/>
       <c r="B52" s="8" t="s">
         <v>25</v>
       </c>
@@ -2419,7 +2422,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="8" t="s">
         <v>14</v>
       </c>
@@ -2430,7 +2433,7 @@
       <c r="E53" s="9"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="8" t="s">
         <v>16</v>
       </c>
@@ -2441,11 +2444,11 @@
       <c r="E54" s="9"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>128</v>
+      <c r="A56" s="19" t="s">
+        <v>127</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>10</v>
@@ -2456,31 +2459,31 @@
       <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
+      <c r="A58" s="20"/>
       <c r="B58" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D58" s="11"/>
       <c r="E58" s="12"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
+      <c r="A59" s="20"/>
       <c r="B59" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>23</v>
@@ -2489,7 +2492,7 @@
       <c r="E59" s="12"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
+      <c r="A60" s="20"/>
       <c r="B60" s="8" t="s">
         <v>14</v>
       </c>
@@ -2500,7 +2503,7 @@
       <c r="E60" s="9"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="8" t="s">
         <v>16</v>
       </c>
@@ -2511,11 +2514,11 @@
       <c r="E61" s="9"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
-        <v>139</v>
+      <c r="A63" s="19" t="s">
+        <v>137</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>10</v>
@@ -2526,64 +2529,64 @@
       <c r="E63" s="9"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>55</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="12" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
+      <c r="A65" s="20"/>
       <c r="B65" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="12"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
+      <c r="A66" s="20"/>
       <c r="B66" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="12"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
+      <c r="A67" s="20"/>
       <c r="B67" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D67" s="11"/>
       <c r="E67" s="12"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
+      <c r="A68" s="20"/>
       <c r="B68" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D68" s="11"/>
       <c r="E68" s="12"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="8" t="s">
         <v>14</v>
       </c>
@@ -2594,7 +2597,7 @@
       <c r="E69" s="9"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="8" t="s">
         <v>16</v>
       </c>
@@ -2606,17 +2609,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A56:A61"/>
-    <mergeCell ref="A63:A70"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A50:A54"/>
     <mergeCell ref="G2:G19"/>
     <mergeCell ref="G36:G40"/>
     <mergeCell ref="G42:G46"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="G21:G34"/>
     <mergeCell ref="A21:A33"/>
+    <mergeCell ref="A56:A61"/>
+    <mergeCell ref="A63:A70"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A50:A54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2676,7 +2679,7 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="21"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
@@ -2693,7 +2696,7 @@
         <v>92</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="21"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
@@ -2710,7 +2713,7 @@
         <v>62</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="21"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
@@ -2727,7 +2730,7 @@
         <v>107</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
@@ -2740,7 +2743,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
@@ -2753,7 +2756,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
@@ -2766,7 +2769,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
@@ -2779,7 +2782,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
@@ -2792,7 +2795,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
@@ -2805,7 +2808,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
@@ -2818,7 +2821,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -2831,7 +2834,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="21"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
@@ -2844,7 +2847,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
@@ -2857,7 +2860,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>